<commit_message>
EHB 311E EHB 311E için önşart eklendi
</commit_message>
<xml_diff>
--- a/Ders Planı.xlsx
+++ b/Ders Planı.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\osman\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\osman\Desktop\Ders-Plani\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -617,7 +617,7 @@
     <cellStyle name="Köprü" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="50">
+  <dxfs count="27">
     <dxf>
       <fill>
         <patternFill>
@@ -636,167 +636,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1246,8 +1085,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="O27" sqref="O27"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2496,117 +2335,122 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="S3:S9 S16:S21 M3:M8">
-    <cfRule type="expression" dxfId="25" priority="21">
+    <cfRule type="expression" dxfId="26" priority="22">
       <formula>IF(Q3=0,TRUE,FALSE)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="24" priority="22">
+    <cfRule type="expression" dxfId="25" priority="23">
       <formula>IF(AND(Q3&gt;0, Q3&lt;2), TRUE, FALSE)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="23" priority="23">
+    <cfRule type="expression" dxfId="24" priority="24">
       <formula>Q3&gt;=2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H20">
-    <cfRule type="expression" dxfId="22" priority="8">
+    <cfRule type="expression" dxfId="23" priority="9">
       <formula>IF($E$9=0,TRUE,FALSE)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T6">
-    <cfRule type="expression" dxfId="21" priority="30">
+    <cfRule type="expression" dxfId="22" priority="31">
       <formula>IF($K$5=0,TRUE,FALSE)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N5 T3">
-    <cfRule type="expression" dxfId="20" priority="31">
+    <cfRule type="expression" dxfId="21" priority="32">
       <formula>IF($K$4=0,TRUE,FALSE)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T7">
-    <cfRule type="expression" dxfId="19" priority="33">
+    <cfRule type="expression" dxfId="20" priority="34">
       <formula>IF($K$3=0,TRUE,FALSE)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B21 T4:T5">
-    <cfRule type="expression" dxfId="18" priority="40">
+    <cfRule type="expression" dxfId="19" priority="41">
       <formula>IF($Q$4=0,TRUE,FALSE)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B16 H17">
-    <cfRule type="expression" dxfId="17" priority="43">
+    <cfRule type="expression" dxfId="18" priority="44">
       <formula>IF($Q$5=0,TRUE,FALSE)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H21">
-    <cfRule type="expression" dxfId="16" priority="45">
+    <cfRule type="expression" dxfId="17" priority="46">
       <formula>IF($Q$8=0,TRUE,FALSE)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B18 H16">
-    <cfRule type="expression" dxfId="15" priority="52">
+    <cfRule type="expression" dxfId="16" priority="53">
       <formula>IF($W$4=0,TRUE,FALSE)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B20 N17">
-    <cfRule type="expression" dxfId="14" priority="54">
+    <cfRule type="expression" dxfId="15" priority="55">
       <formula>IF($W$3=0,TRUE,FALSE)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H18">
-    <cfRule type="expression" dxfId="13" priority="61">
+    <cfRule type="expression" dxfId="14" priority="62">
       <formula>IF($E$16=0,TRUE,FALSE)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A16:A23 A3:A10 G3:G8">
-    <cfRule type="expression" dxfId="12" priority="62">
+    <cfRule type="expression" dxfId="13" priority="63">
       <formula>IF(E3=0,TRUE,FALSE)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="11" priority="63">
+    <cfRule type="expression" dxfId="12" priority="64">
       <formula>IF(AND(E3&gt;0, E3&lt;2), TRUE, FALSE)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="64">
+    <cfRule type="expression" dxfId="11" priority="65">
       <formula>E3&gt;=2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G16:G23">
-    <cfRule type="expression" dxfId="9" priority="65">
+    <cfRule type="expression" dxfId="10" priority="66">
       <formula>IF(K16=0,TRUE,FALSE)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="8" priority="66">
+    <cfRule type="expression" dxfId="9" priority="67">
       <formula>IF(AND(K16&gt;0, K16&lt;2), TRUE, FALSE)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="7" priority="67">
+    <cfRule type="expression" dxfId="8" priority="68">
       <formula>K16&gt;=2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M16:M22">
-    <cfRule type="expression" dxfId="6" priority="68">
+    <cfRule type="expression" dxfId="7" priority="69">
       <formula>IF(Q16=0,TRUE,FALSE)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="5" priority="69">
+    <cfRule type="expression" dxfId="6" priority="70">
       <formula>IF(AND(Q16&gt;0, Q16&lt;2), TRUE, FALSE)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="70">
+    <cfRule type="expression" dxfId="5" priority="71">
       <formula>Q16&gt;=2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N6">
-    <cfRule type="expression" dxfId="3" priority="4">
+    <cfRule type="expression" dxfId="4" priority="5">
       <formula>IF($E$9=0,TRUE,FALSE)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N8">
-    <cfRule type="expression" dxfId="2" priority="3">
+    <cfRule type="expression" dxfId="3" priority="4">
       <formula>IF($K$8=0,TRUE,FALSE)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H5">
-    <cfRule type="expression" dxfId="1" priority="2">
+    <cfRule type="expression" dxfId="2" priority="3">
       <formula>IF($E$8=0,TRUE,FALSE)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N3">
+    <cfRule type="expression" dxfId="1" priority="2">
+      <formula>IF($K$5=0,TRUE,FALSE)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B22">
     <cfRule type="expression" dxfId="0" priority="1">
-      <formula>IF($K$5=0,TRUE,FALSE)</formula>
+      <formula>IF($Q$6=0,TRUE,FALSE)</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>

</xml_diff>